<commit_message>
change order of experiments within files
</commit_message>
<xml_diff>
--- a/ExperimentalData/ChangeRHO/ChangeRHO_G238S.xlsx
+++ b/ExperimentalData/ChangeRHO/ChangeRHO_G238S.xlsx
@@ -5,19 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Plate design 1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Plate design 2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="G238S None 1" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="G238S None 2" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="G238S High 1" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="G238S High 2" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="G238S Low 1" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="G238S Low 2" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="G238S Med 1" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="G238S Med 2" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="G238S Low 1" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="G238S Low 2" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="G238S High 1" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="G238S High 2" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -273,7 +273,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -283,10 +283,7 @@
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.77"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D1" s="0" t="s">
@@ -1120,8 +1117,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1130,7 +1127,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -1140,10 +1137,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">
@@ -1188,40 +1182,40 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="n">
-        <v>0.431903793247937</v>
+        <v>0.438400198234548</v>
       </c>
       <c r="C2" s="5" t="n">
-        <v>0.504987096947535</v>
+        <v>0.244484268780024</v>
       </c>
       <c r="D2" s="5" t="n">
-        <v>0.502364982207096</v>
+        <v>0.224334482274559</v>
       </c>
       <c r="E2" s="5" t="n">
-        <v>0.48863882663303</v>
+        <v>0.448518905041597</v>
       </c>
       <c r="F2" s="5" t="n">
-        <v>0.487708690533728</v>
+        <v>0.51859159553502</v>
       </c>
       <c r="G2" s="5" t="n">
-        <v>0.442115759501721</v>
+        <v>0.218054531233898</v>
       </c>
       <c r="H2" s="5" t="n">
-        <v>0.48399962543033</v>
+        <v>0.605886370308883</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>0.520628587307968</v>
+        <v>0.205051242448784</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>0.458624959752355</v>
+        <v>0.202433910904375</v>
       </c>
       <c r="K2" s="5" t="n">
-        <v>0.480150521224239</v>
+        <v>0.280153859015398</v>
       </c>
       <c r="L2" s="5" t="n">
-        <v>0.478247712263137</v>
+        <v>0.227565771888255</v>
       </c>
       <c r="M2" s="5" t="n">
-        <v>0.459817095543563</v>
+        <v>0.230366332314481</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,40 +1223,40 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="n">
-        <v>0.0408427011528876</v>
+        <v>0.193982844235816</v>
       </c>
       <c r="C3" s="5" t="n">
-        <v>0.0407150509417079</v>
+        <v>0.199282130171143</v>
       </c>
       <c r="D3" s="5" t="n">
-        <v>0.0765181307385421</v>
+        <v>0.204948372652862</v>
       </c>
       <c r="E3" s="5" t="n">
-        <v>0.291034565593748</v>
+        <v>0.196078749008882</v>
       </c>
       <c r="F3" s="5" t="n">
-        <v>0.514252881822799</v>
+        <v>0.592892868415679</v>
       </c>
       <c r="G3" s="5" t="n">
-        <v>0.464932038814978</v>
+        <v>0.570360144996179</v>
       </c>
       <c r="H3" s="5" t="n">
-        <v>0.517996923290498</v>
+        <v>0.209656436528331</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>0.484423868708474</v>
+        <v>0.623190568449295</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>0.547395465196192</v>
+        <v>0.136607648633037</v>
       </c>
       <c r="K3" s="5" t="n">
-        <v>0.521739058352267</v>
+        <v>0.155806316849541</v>
       </c>
       <c r="L3" s="5" t="n">
-        <v>0.483592409137944</v>
+        <v>0.157601158386656</v>
       </c>
       <c r="M3" s="5" t="n">
-        <v>0.427186184140082</v>
+        <v>0.648427523846872</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1270,40 +1264,40 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="n">
-        <v>0.0399260110850138</v>
+        <v>0.0400065210699787</v>
       </c>
       <c r="C4" s="5" t="n">
-        <v>0.0397633526299448</v>
+        <v>0.0398366292390349</v>
       </c>
       <c r="D4" s="5" t="n">
-        <v>0.0391975128961616</v>
+        <v>0.0393862905073723</v>
       </c>
       <c r="E4" s="5" t="n">
-        <v>0.0392721591312438</v>
+        <v>0.0428856905936506</v>
       </c>
       <c r="F4" s="5" t="n">
-        <v>0.0392978404023175</v>
+        <v>0.133130933170056</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>0.0391831822870884</v>
+        <v>0.140763092804546</v>
       </c>
       <c r="H4" s="5" t="n">
-        <v>0.435027066695581</v>
+        <v>0.199533432602947</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>0.352812034567141</v>
+        <v>0.222296675033094</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>0.364183573298967</v>
+        <v>0.340428193882865</v>
       </c>
       <c r="K4" s="5" t="n">
-        <v>0.456066424394761</v>
+        <v>0.161875026639532</v>
       </c>
       <c r="L4" s="5" t="n">
-        <v>0.570097730087717</v>
+        <v>0.579287102753755</v>
       </c>
       <c r="M4" s="5" t="n">
-        <v>0.398548763290113</v>
+        <v>0.160662668015325</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1311,40 +1305,40 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="n">
-        <v>0.039527845057948</v>
+        <v>0.0392011675927911</v>
       </c>
       <c r="C5" s="5" t="n">
-        <v>0.0408079382229739</v>
+        <v>0.0389043023612644</v>
       </c>
       <c r="D5" s="5" t="n">
-        <v>0.0387469222111278</v>
+        <v>0.0385909995288353</v>
       </c>
       <c r="E5" s="5" t="n">
-        <v>0.0383528150077093</v>
+        <v>0.0412651925037234</v>
       </c>
       <c r="F5" s="5" t="n">
-        <v>0.0388167182444321</v>
+        <v>0.0389352287473637</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>0.0387528872456906</v>
+        <v>0.0388293744808296</v>
       </c>
       <c r="H5" s="5" t="n">
-        <v>0.0383534109664211</v>
+        <v>0.368898527155458</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>0.0373735684316622</v>
+        <v>0.248935135712266</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>0.394665231957158</v>
+        <v>0.176065159431614</v>
       </c>
       <c r="K5" s="5" t="n">
-        <v>0.443378448761206</v>
+        <v>0.190460560864515</v>
       </c>
       <c r="L5" s="5" t="n">
-        <v>0.501048596146307</v>
+        <v>0.241755586499667</v>
       </c>
       <c r="M5" s="5" t="n">
-        <v>0.411155366150051</v>
+        <v>0.594373334374918</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1352,40 +1346,40 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="n">
-        <v>0.0394447903649976</v>
+        <v>0.0391482048147441</v>
       </c>
       <c r="C6" s="5" t="n">
-        <v>0.0384279122463169</v>
+        <v>0.0389423659184561</v>
       </c>
       <c r="D6" s="5" t="n">
-        <v>0.0385107726799496</v>
+        <v>0.0391398741791119</v>
       </c>
       <c r="E6" s="5" t="n">
-        <v>0.0379066714753056</v>
+        <v>0.0393428301308367</v>
       </c>
       <c r="F6" s="5" t="n">
-        <v>0.0387159053520393</v>
+        <v>0.0380125482798961</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>0.0385000416607483</v>
+        <v>0.0395560062270268</v>
       </c>
       <c r="H6" s="5" t="n">
-        <v>0.0384475827167735</v>
+        <v>0.363637412222159</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>0.0388155250556078</v>
+        <v>0.22158601249534</v>
       </c>
       <c r="J6" s="5" t="n">
-        <v>0.56594505294746</v>
+        <v>0.702283224627248</v>
       </c>
       <c r="K6" s="5" t="n">
-        <v>0.555855459686953</v>
+        <v>0.173261264622959</v>
       </c>
       <c r="L6" s="5" t="n">
-        <v>0.492118425534917</v>
+        <v>0.201736823452209</v>
       </c>
       <c r="M6" s="5" t="n">
-        <v>0.414159333480472</v>
+        <v>0.253232337628753</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,40 +1387,40 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="n">
-        <v>0.0399798453139494</v>
+        <v>0.0387039289568339</v>
       </c>
       <c r="C7" s="5" t="n">
-        <v>0.0392058726365018</v>
+        <v>0.0385814910226718</v>
       </c>
       <c r="D7" s="5" t="n">
-        <v>0.0388047865037047</v>
+        <v>0.0386997678779135</v>
       </c>
       <c r="E7" s="5" t="n">
-        <v>0.0386980120178559</v>
+        <v>0.0387931045156367</v>
       </c>
       <c r="F7" s="5" t="n">
-        <v>0.0383188467128953</v>
+        <v>0.0393035409308845</v>
       </c>
       <c r="G7" s="5" t="n">
-        <v>0.0387033799407031</v>
+        <v>0.0386355734267507</v>
       </c>
       <c r="H7" s="5" t="n">
-        <v>0.0387648175606113</v>
+        <v>0.0391946212816369</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>0.038712923078479</v>
+        <v>0.596287915868336</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>0.0387105372743756</v>
+        <v>0.174736154152166</v>
       </c>
       <c r="K7" s="5" t="n">
-        <v>0.42143231948562</v>
+        <v>0.200670412165766</v>
       </c>
       <c r="L7" s="5" t="n">
-        <v>0.403774510556357</v>
+        <v>0.613188547166689</v>
       </c>
       <c r="M7" s="5" t="n">
-        <v>0.394546121084357</v>
+        <v>0.632060502603721</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1434,40 +1428,40 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="n">
-        <v>0.0394985649721716</v>
+        <v>0.0388864612171669</v>
       </c>
       <c r="C8" s="5" t="n">
-        <v>0.0385853009617529</v>
+        <v>0.0383824544703029</v>
       </c>
       <c r="D8" s="5" t="n">
-        <v>0.0383206344516504</v>
+        <v>0.0390006572064271</v>
       </c>
       <c r="E8" s="5" t="n">
-        <v>0.038980216109897</v>
+        <v>0.0385618803861617</v>
       </c>
       <c r="F8" s="5" t="n">
-        <v>0.0384434101182877</v>
+        <v>0.0385636631347076</v>
       </c>
       <c r="G8" s="5" t="n">
-        <v>0.0385853009617529</v>
+        <v>0.0385262269519488</v>
       </c>
       <c r="H8" s="5" t="n">
-        <v>0.0409518028983176</v>
+        <v>0.0388513757717435</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>0.0385602580323317</v>
+        <v>0.212857177074666</v>
       </c>
       <c r="J8" s="5" t="n">
-        <v>0.0380936504893584</v>
+        <v>0.301917227688681</v>
       </c>
       <c r="K8" s="5" t="n">
-        <v>0.433162241958568</v>
+        <v>0.638900777986526</v>
       </c>
       <c r="L8" s="5" t="n">
-        <v>0.428021523365581</v>
+        <v>0.586607261067464</v>
       </c>
       <c r="M8" s="5" t="n">
-        <v>0.435821081006658</v>
+        <v>0.181438741864025</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1475,40 +1469,40 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="n">
-        <v>0.0392870899180009</v>
+        <v>0.0376886196895793</v>
       </c>
       <c r="C9" s="5" t="n">
-        <v>0.0383611585040946</v>
+        <v>0.0383420641556675</v>
       </c>
       <c r="D9" s="5" t="n">
-        <v>0.0379775234759788</v>
+        <v>0.0387669444538546</v>
       </c>
       <c r="E9" s="5" t="n">
-        <v>0.0377965463550024</v>
+        <v>0.0381787592739534</v>
       </c>
       <c r="F9" s="5" t="n">
-        <v>0.0379150064048739</v>
+        <v>0.0398193457248754</v>
       </c>
       <c r="G9" s="5" t="n">
-        <v>0.0379888370504755</v>
+        <v>0.0380914905705733</v>
       </c>
       <c r="H9" s="5" t="n">
-        <v>0.0378655945164244</v>
+        <v>0.0382013213833845</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>0.0380406450774416</v>
+        <v>0.233492154514637</v>
       </c>
       <c r="J9" s="5" t="n">
-        <v>0.0380001509197037</v>
+        <v>0.697035818730515</v>
       </c>
       <c r="K9" s="5" t="n">
-        <v>0.557877184793937</v>
+        <v>0.202051023758154</v>
       </c>
       <c r="L9" s="5" t="n">
-        <v>0.554181106055787</v>
+        <v>0.23458546313071</v>
       </c>
       <c r="M9" s="5" t="n">
-        <v>0.743111026404603</v>
+        <v>0.255547298818602</v>
       </c>
     </row>
   </sheetData>
@@ -1533,8 +1527,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1543,20 +1537,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="C1:T22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.77"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="16.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D1" s="0" t="s">
@@ -2390,8 +2381,8 @@
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2400,7 +2391,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2410,10 +2401,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">
@@ -2803,8 +2791,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2813,7 +2801,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -2823,10 +2811,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">
@@ -3216,8 +3201,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3226,7 +3211,1647 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>0.338153373460269</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>0.554603883751092</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0.537996591121118</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>0.514096797160892</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>0.50217268346036</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>0.479205865183706</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <v>0.646437906025183</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>0.376440385611703</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <v>0.558790202009899</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>0.540711838342408</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <v>0.569482927239416</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <v>0.477927138475242</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.0408012989152388</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.0413836721194609</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0.0423398763721745</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0.181624646010517</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0.377321287871159</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>0.52981533733745</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>0.526889734923352</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>0.5419849143909</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>0.507616012759637</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <v>0.3964904369002</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>0.415487840806478</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <v>0.540622137454392</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0.0399677628324548</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0.0402287493324903</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0.0393782577331568</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.0391105651657672</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0.0387264590222155</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0.0377433976524823</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>0.0400213939049781</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>0.11748191877229</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>0.286412601090833</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>0.400712131636769</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>0.526715969805007</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>0.463132419395305</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0.0399882503255867</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0.0381218348861506</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0.0413449841265705</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0.0394570930591579</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0.0411352826437749</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>0.0390630594571304</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>0.0384087312666514</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>0.0388803011367327</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>0.464744663217354</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>0.460906251430879</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>0.505162728791778</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <v>0.494961601003546</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>0.0435387074468432</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0.0394276033611212</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.0374413643675347</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.0376450939239616</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0.0369671646161863</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0.0390257801350154</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0.0378777021214141</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>0.0392982334516857</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>0.209296995440488</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>0.481047016824626</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>0.582657833930603</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <v>0.466313056903085</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>0.0409413837821215</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0.0388905191445103</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.0396099901257659</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.0381410354203052</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0.0379328749199118</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0.0383631032693955</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>0.0394077440805766</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>0.040038870628971</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <v>0.039550991966244</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <v>0.505699467364757</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>0.508139856208004</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <v>0.476411775592257</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>0.041343775182324</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>0.0397009111447857</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.0400316387958135</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>0.0391213899782058</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>0.0383024734800633</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>0.0397816119664764</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>0.0390155589443817</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>0.0397328283338832</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>0.46651734864765</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>0.496083107326997</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <v>0.50731367468521</v>
+      </c>
+      <c r="M8" s="5" t="n">
+        <v>0.545987018735033</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>0.0386795960826078</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0.0397707706856615</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>0.038533031837442</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>0.0387577037915165</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>0.038402126917703</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>0.0379256780704267</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>0.0394992246731085</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>0.0387240556715275</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>0.0386795960826078</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>0.579645234104184</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <v>0.555661502821253</v>
+      </c>
+      <c r="M9" s="5" t="n">
+        <v>0.682762942722486</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:M9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>0.431903793247937</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>0.504987096947535</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0.502364982207096</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>0.48863882663303</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>0.487708690533728</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>0.442115759501721</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <v>0.48399962543033</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>0.520628587307968</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <v>0.458624959752355</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>0.480150521224239</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <v>0.478247712263137</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <v>0.459817095543563</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.0408427011528876</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.0407150509417079</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0.0765181307385421</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0.291034565593748</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0.514252881822799</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>0.464932038814978</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>0.517996923290498</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>0.484423868708474</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>0.547395465196192</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <v>0.521739058352267</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>0.483592409137944</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <v>0.427186184140082</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0.0399260110850138</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0.0397633526299448</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0.0391975128961616</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.0392721591312438</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0.0392978404023175</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0.0391831822870884</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>0.435027066695581</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>0.352812034567141</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>0.364183573298967</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>0.456066424394761</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>0.570097730087717</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>0.398548763290113</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0.039527845057948</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0.0408079382229739</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0.0387469222111278</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0.0383528150077093</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0.0388167182444321</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>0.0387528872456906</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>0.0383534109664211</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>0.0373735684316622</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>0.394665231957158</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>0.443378448761206</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>0.501048596146307</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <v>0.411155366150051</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>0.0394447903649976</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0.0384279122463169</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.0385107726799496</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.0379066714753056</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0.0387159053520393</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0.0385000416607483</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0.0384475827167735</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>0.0388155250556078</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>0.56594505294746</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>0.555855459686953</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>0.492118425534917</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <v>0.414159333480472</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>0.0399798453139494</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0.0392058726365018</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.0388047865037047</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.0386980120178559</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0.0383188467128953</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0.0387033799407031</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>0.0387648175606113</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>0.038712923078479</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <v>0.0387105372743756</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <v>0.42143231948562</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>0.403774510556357</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <v>0.394546121084357</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>0.0394985649721716</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>0.0385853009617529</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.0383206344516504</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>0.038980216109897</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>0.0384434101182877</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>0.0385853009617529</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>0.0409518028983176</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>0.0385602580323317</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>0.0380936504893584</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>0.433162241958568</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <v>0.428021523365581</v>
+      </c>
+      <c r="M8" s="5" t="n">
+        <v>0.435821081006658</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>0.0392870899180009</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0.0383611585040946</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>0.0379775234759788</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>0.0377965463550024</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>0.0379150064048739</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>0.0379888370504755</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>0.0378655945164244</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>0.0380406450774416</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>0.0380001509197037</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>0.557877184793937</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <v>0.554181106055787</v>
+      </c>
+      <c r="M9" s="5" t="n">
+        <v>0.743111026404603</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:M9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>0.476160959679535</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>0.355696974751736</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0.394955394428143</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>0.398101902841471</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>0.415130381706406</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>0.386071151149093</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <v>0.401187489404748</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>0.370074885867138</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <v>0.375199288025577</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>0.52651920479026</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <v>0.359335411341877</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <v>0.426012771703021</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.041061167948131</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.33917334811026</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0.393246836328295</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0.447088159756565</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0.426825937411241</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>0.34744587407625</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>0.354336986820816</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>0.508440307188054</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>0.307449129912469</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <v>0.295860492239587</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>0.330490721521082</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <v>0.310663372630102</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0.0395720021184361</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0.0402662309167242</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0.0394667677455208</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.0400656284363337</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0.0396443655443304</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0.041940529386311</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>0.185237077700105</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>0.334808566549055</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>0.260720267456683</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>0.297432070514934</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>0.403517534150972</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>0.279409741085279</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0.0392014033729497</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0.0393095616155426</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0.0390622116878799</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0.039015028065797</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0.0395295465471985</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>0.0388657465763251</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>0.039497259172901</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>0.31964828721026</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>0.295145761974993</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>0.324181483554502</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>0.451036890848853</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <v>0.316270976065301</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>0.039427311428827</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0.0393119521571886</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.0387767992073567</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.0398423800147353</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0.0386264061781014</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0.0399884062145222</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0.0380438266581138</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>0.350316634436598</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>0.320228759963691</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>0.330134485364631</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>0.370580769308719</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <v>0.541253978201313</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>0.0396712806384341</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0.0392169382594484</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.0386001524174543</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.0397873336999042</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0.0385971691359822</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0.0401410680505095</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>0.0380384636405363</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>0.0382852310195775</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <v>0.450831816398439</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <v>0.380750722967372</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>0.440205944430658</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <v>0.389208558681117</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>0.0428795175179015</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>0.0388191812519952</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.0400380902549119</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>0.0385506325982476</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>0.0390861040844676</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>0.0387905281492044</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>0.0388938075800053</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>0.038970238230841</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>0.239382873023121</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>0.363061260097311</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <v>0.307609832565581</v>
+      </c>
+      <c r="M8" s="5" t="n">
+        <v>0.525767490656375</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>0.0386431139430636</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0.0391816868172169</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>0.0393053781993247</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>0.0389606836638589</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>0.0384134384980871</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>0.0386616125754874</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>0.0382965594583559</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>0.0369772943339069</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>0.396515596522007</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>0.408344051148392</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <v>0.369142787285043</v>
+      </c>
+      <c r="M9" s="5" t="n">
+        <v>0.502854257860951</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:M9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>0.423538992639194</v>
+      </c>
+      <c r="C2" s="5" t="n">
+        <v>0.488311732314396</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>0.451994938393242</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>0.612125962396808</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>0.505562872328129</v>
+      </c>
+      <c r="G2" s="5" t="n">
+        <v>0.486014862353483</v>
+      </c>
+      <c r="H2" s="5" t="n">
+        <v>0.482174833113015</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>0.288064182715374</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <v>0.45236798978276</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>0.304945047879883</v>
+      </c>
+      <c r="L2" s="5" t="n">
+        <v>0.360645035553213</v>
+      </c>
+      <c r="M2" s="5" t="n">
+        <v>0.335097450693683</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>0.0440370781706982</v>
+      </c>
+      <c r="C3" s="5" t="n">
+        <v>0.368373889678204</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>0.458892991087051</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>0.450014318771457</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>0.588153206280568</v>
+      </c>
+      <c r="G3" s="5" t="n">
+        <v>0.362233947914272</v>
+      </c>
+      <c r="H3" s="5" t="n">
+        <v>0.378085637290039</v>
+      </c>
+      <c r="I3" s="5" t="n">
+        <v>0.337842755332675</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>0.503218447489921</v>
+      </c>
+      <c r="K3" s="5" t="n">
+        <v>0.285926631609546</v>
+      </c>
+      <c r="L3" s="5" t="n">
+        <v>0.287204723238003</v>
+      </c>
+      <c r="M3" s="5" t="n">
+        <v>0.41506363499817</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>0.0397413759440207</v>
+      </c>
+      <c r="C4" s="5" t="n">
+        <v>0.0394474444902204</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>0.039533627805454</v>
+      </c>
+      <c r="E4" s="5" t="n">
+        <v>0.0395503876585529</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>0.0384348754692067</v>
+      </c>
+      <c r="G4" s="5" t="n">
+        <v>0.0400103388324699</v>
+      </c>
+      <c r="H4" s="5" t="n">
+        <v>0.399512601407442</v>
+      </c>
+      <c r="I4" s="5" t="n">
+        <v>0.394140913435524</v>
+      </c>
+      <c r="J4" s="5" t="n">
+        <v>0.395436188276863</v>
+      </c>
+      <c r="K4" s="5" t="n">
+        <v>0.34506888821952</v>
+      </c>
+      <c r="L4" s="5" t="n">
+        <v>0.34397920405824</v>
+      </c>
+      <c r="M4" s="5" t="n">
+        <v>0.5188012073911</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>0.0404995712871189</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>0.0395934873938042</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0.0399953587906389</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>0.0392763255491709</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0.0385429535581762</v>
+      </c>
+      <c r="G5" s="5" t="n">
+        <v>0.0391830163553665</v>
+      </c>
+      <c r="H5" s="5" t="n">
+        <v>0.0394414601728049</v>
+      </c>
+      <c r="I5" s="5" t="n">
+        <v>0.254641566609901</v>
+      </c>
+      <c r="J5" s="5" t="n">
+        <v>0.409880561097697</v>
+      </c>
+      <c r="K5" s="5" t="n">
+        <v>0.563664357071781</v>
+      </c>
+      <c r="L5" s="5" t="n">
+        <v>0.351883699201556</v>
+      </c>
+      <c r="M5" s="5" t="n">
+        <v>0.290367979633172</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>0.0397341899111802</v>
+      </c>
+      <c r="C6" s="5" t="n">
+        <v>0.0385501199071268</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0.0372924464949003</v>
+      </c>
+      <c r="E6" s="5" t="n">
+        <v>0.0387096017657734</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>0.0381549528984127</v>
+      </c>
+      <c r="G6" s="5" t="n">
+        <v>0.0397467655466825</v>
+      </c>
+      <c r="H6" s="5" t="n">
+        <v>0.296383672111385</v>
+      </c>
+      <c r="I6" s="5" t="n">
+        <v>0.339298925104208</v>
+      </c>
+      <c r="J6" s="5" t="n">
+        <v>0.405547605714917</v>
+      </c>
+      <c r="K6" s="5" t="n">
+        <v>0.378227920430886</v>
+      </c>
+      <c r="L6" s="5" t="n">
+        <v>0.392125001485235</v>
+      </c>
+      <c r="M6" s="5" t="n">
+        <v>0.484204735815363</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>0.0402380991078626</v>
+      </c>
+      <c r="C7" s="5" t="n">
+        <v>0.0381155752870734</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0.0394025641194448</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>0.0391537118353301</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>0.0398509776802667</v>
+      </c>
+      <c r="G7" s="5" t="n">
+        <v>0.0395402119563223</v>
+      </c>
+      <c r="H7" s="5" t="n">
+        <v>0.0392302665825735</v>
+      </c>
+      <c r="I7" s="5" t="n">
+        <v>0.0413107763048406</v>
+      </c>
+      <c r="J7" s="5" t="n">
+        <v>0.381049249143666</v>
+      </c>
+      <c r="K7" s="5" t="n">
+        <v>0.601778101815888</v>
+      </c>
+      <c r="L7" s="5" t="n">
+        <v>0.464239253219776</v>
+      </c>
+      <c r="M7" s="5" t="n">
+        <v>0.348848327890818</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>0.0392745309525255</v>
+      </c>
+      <c r="C8" s="5" t="n">
+        <v>0.0394366727782432</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>0.039213519078473</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>0.0388488229424941</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>0.0392326591358807</v>
+      </c>
+      <c r="G8" s="5" t="n">
+        <v>0.0392428276344861</v>
+      </c>
+      <c r="H8" s="5" t="n">
+        <v>0.0396677247435611</v>
+      </c>
+      <c r="I8" s="5" t="n">
+        <v>0.0388769115942524</v>
+      </c>
+      <c r="J8" s="5" t="n">
+        <v>0.589102664878692</v>
+      </c>
+      <c r="K8" s="5" t="n">
+        <v>0.383648362595784</v>
+      </c>
+      <c r="L8" s="5" t="n">
+        <v>0.426899464737079</v>
+      </c>
+      <c r="M8" s="5" t="n">
+        <v>0.427136112806911</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>0.0377213993574357</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>0.0400229224669291</v>
+      </c>
+      <c r="D9" s="5" t="n">
+        <v>0.0405295666929271</v>
+      </c>
+      <c r="E9" s="5" t="n">
+        <v>0.0384856270232751</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>0.038568633522598</v>
+      </c>
+      <c r="G9" s="5" t="n">
+        <v>0.0387048224319293</v>
+      </c>
+      <c r="H9" s="5" t="n">
+        <v>0.0387257324058124</v>
+      </c>
+      <c r="I9" s="5" t="n">
+        <v>0.0390526563117933</v>
+      </c>
+      <c r="J9" s="5" t="n">
+        <v>0.446034185730248</v>
+      </c>
+      <c r="K9" s="5" t="n">
+        <v>0.432144613186851</v>
+      </c>
+      <c r="L9" s="5" t="n">
+        <v>0.471834721759773</v>
+      </c>
+      <c r="M9" s="5" t="n">
+        <v>0.746237781267078</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:M9">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -3236,10 +4861,7 @@
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="n">
@@ -3632,1660 +5254,8 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M9"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>0.438400198234548</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>0.244484268780024</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>0.224334482274559</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>0.448518905041597</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>0.51859159553502</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>0.218054531233898</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <v>0.605886370308883</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>0.205051242448784</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <v>0.202433910904375</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>0.280153859015398</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>0.227565771888255</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>0.230366332314481</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>0.193982844235816</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>0.199282130171143</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>0.204948372652862</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>0.196078749008882</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>0.592892868415679</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>0.570360144996179</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>0.209656436528331</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>0.623190568449295</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <v>0.136607648633037</v>
-      </c>
-      <c r="K3" s="5" t="n">
-        <v>0.155806316849541</v>
-      </c>
-      <c r="L3" s="5" t="n">
-        <v>0.157601158386656</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>0.648427523846872</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>0.0400065210699787</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0.0398366292390349</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>0.0393862905073723</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>0.0428856905936506</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0.133130933170056</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>0.140763092804546</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>0.199533432602947</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>0.222296675033094</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>0.340428193882865</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>0.161875026639532</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <v>0.579287102753755</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>0.160662668015325</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>0.0392011675927911</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0.0389043023612644</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>0.0385909995288353</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>0.0412651925037234</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0.0389352287473637</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>0.0388293744808296</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>0.368898527155458</v>
-      </c>
-      <c r="I5" s="5" t="n">
-        <v>0.248935135712266</v>
-      </c>
-      <c r="J5" s="5" t="n">
-        <v>0.176065159431614</v>
-      </c>
-      <c r="K5" s="5" t="n">
-        <v>0.190460560864515</v>
-      </c>
-      <c r="L5" s="5" t="n">
-        <v>0.241755586499667</v>
-      </c>
-      <c r="M5" s="5" t="n">
-        <v>0.594373334374918</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>0.0391482048147441</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>0.0389423659184561</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>0.0391398741791119</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>0.0393428301308367</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>0.0380125482798961</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>0.0395560062270268</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>0.363637412222159</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <v>0.22158601249534</v>
-      </c>
-      <c r="J6" s="5" t="n">
-        <v>0.702283224627248</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>0.173261264622959</v>
-      </c>
-      <c r="L6" s="5" t="n">
-        <v>0.201736823452209</v>
-      </c>
-      <c r="M6" s="5" t="n">
-        <v>0.253232337628753</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>0.0387039289568339</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>0.0385814910226718</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>0.0386997678779135</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>0.0387931045156367</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>0.0393035409308845</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <v>0.0386355734267507</v>
-      </c>
-      <c r="H7" s="5" t="n">
-        <v>0.0391946212816369</v>
-      </c>
-      <c r="I7" s="5" t="n">
-        <v>0.596287915868336</v>
-      </c>
-      <c r="J7" s="5" t="n">
-        <v>0.174736154152166</v>
-      </c>
-      <c r="K7" s="5" t="n">
-        <v>0.200670412165766</v>
-      </c>
-      <c r="L7" s="5" t="n">
-        <v>0.613188547166689</v>
-      </c>
-      <c r="M7" s="5" t="n">
-        <v>0.632060502603721</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>0.0388864612171669</v>
-      </c>
-      <c r="C8" s="5" t="n">
-        <v>0.0383824544703029</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>0.0390006572064271</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>0.0385618803861617</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>0.0385636631347076</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>0.0385262269519488</v>
-      </c>
-      <c r="H8" s="5" t="n">
-        <v>0.0388513757717435</v>
-      </c>
-      <c r="I8" s="5" t="n">
-        <v>0.212857177074666</v>
-      </c>
-      <c r="J8" s="5" t="n">
-        <v>0.301917227688681</v>
-      </c>
-      <c r="K8" s="5" t="n">
-        <v>0.638900777986526</v>
-      </c>
-      <c r="L8" s="5" t="n">
-        <v>0.586607261067464</v>
-      </c>
-      <c r="M8" s="5" t="n">
-        <v>0.181438741864025</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>0.0376886196895793</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>0.0383420641556675</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>0.0387669444538546</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>0.0381787592739534</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>0.0398193457248754</v>
-      </c>
-      <c r="G9" s="5" t="n">
-        <v>0.0380914905705733</v>
-      </c>
-      <c r="H9" s="5" t="n">
-        <v>0.0382013213833845</v>
-      </c>
-      <c r="I9" s="5" t="n">
-        <v>0.233492154514637</v>
-      </c>
-      <c r="J9" s="5" t="n">
-        <v>0.697035818730515</v>
-      </c>
-      <c r="K9" s="5" t="n">
-        <v>0.202051023758154</v>
-      </c>
-      <c r="L9" s="5" t="n">
-        <v>0.23458546313071</v>
-      </c>
-      <c r="M9" s="5" t="n">
-        <v>0.255547298818602</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:M9">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M9"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>0.476160959679535</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>0.355696974751736</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>0.394955394428143</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>0.398101902841471</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>0.415130381706406</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>0.386071151149093</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <v>0.401187489404748</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>0.370074885867138</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <v>0.375199288025577</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>0.52651920479026</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>0.359335411341877</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>0.426012771703021</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>0.041061167948131</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>0.33917334811026</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>0.393246836328295</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>0.447088159756565</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>0.426825937411241</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>0.34744587407625</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>0.354336986820816</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>0.508440307188054</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <v>0.307449129912469</v>
-      </c>
-      <c r="K3" s="5" t="n">
-        <v>0.295860492239587</v>
-      </c>
-      <c r="L3" s="5" t="n">
-        <v>0.330490721521082</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>0.310663372630102</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>0.0395720021184361</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0.0402662309167242</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>0.0394667677455208</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>0.0400656284363337</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0.0396443655443304</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>0.041940529386311</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>0.185237077700105</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>0.334808566549055</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>0.260720267456683</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>0.297432070514934</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <v>0.403517534150972</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>0.279409741085279</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>0.0392014033729497</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0.0393095616155426</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>0.0390622116878799</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>0.039015028065797</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0.0395295465471985</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>0.0388657465763251</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>0.039497259172901</v>
-      </c>
-      <c r="I5" s="5" t="n">
-        <v>0.31964828721026</v>
-      </c>
-      <c r="J5" s="5" t="n">
-        <v>0.295145761974993</v>
-      </c>
-      <c r="K5" s="5" t="n">
-        <v>0.324181483554502</v>
-      </c>
-      <c r="L5" s="5" t="n">
-        <v>0.451036890848853</v>
-      </c>
-      <c r="M5" s="5" t="n">
-        <v>0.316270976065301</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>0.039427311428827</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>0.0393119521571886</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>0.0387767992073567</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>0.0398423800147353</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>0.0386264061781014</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>0.0399884062145222</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>0.0380438266581138</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <v>0.350316634436598</v>
-      </c>
-      <c r="J6" s="5" t="n">
-        <v>0.320228759963691</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>0.330134485364631</v>
-      </c>
-      <c r="L6" s="5" t="n">
-        <v>0.370580769308719</v>
-      </c>
-      <c r="M6" s="5" t="n">
-        <v>0.541253978201313</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>0.0396712806384341</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>0.0392169382594484</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>0.0386001524174543</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>0.0397873336999042</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>0.0385971691359822</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <v>0.0401410680505095</v>
-      </c>
-      <c r="H7" s="5" t="n">
-        <v>0.0380384636405363</v>
-      </c>
-      <c r="I7" s="5" t="n">
-        <v>0.0382852310195775</v>
-      </c>
-      <c r="J7" s="5" t="n">
-        <v>0.450831816398439</v>
-      </c>
-      <c r="K7" s="5" t="n">
-        <v>0.380750722967372</v>
-      </c>
-      <c r="L7" s="5" t="n">
-        <v>0.440205944430658</v>
-      </c>
-      <c r="M7" s="5" t="n">
-        <v>0.389208558681117</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>0.0428795175179015</v>
-      </c>
-      <c r="C8" s="5" t="n">
-        <v>0.0388191812519952</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>0.0400380902549119</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>0.0385506325982476</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>0.0390861040844676</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>0.0387905281492044</v>
-      </c>
-      <c r="H8" s="5" t="n">
-        <v>0.0388938075800053</v>
-      </c>
-      <c r="I8" s="5" t="n">
-        <v>0.038970238230841</v>
-      </c>
-      <c r="J8" s="5" t="n">
-        <v>0.239382873023121</v>
-      </c>
-      <c r="K8" s="5" t="n">
-        <v>0.363061260097311</v>
-      </c>
-      <c r="L8" s="5" t="n">
-        <v>0.307609832565581</v>
-      </c>
-      <c r="M8" s="5" t="n">
-        <v>0.525767490656375</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>0.0386431139430636</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>0.0391816868172169</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>0.0393053781993247</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>0.0389606836638589</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>0.0384134384980871</v>
-      </c>
-      <c r="G9" s="5" t="n">
-        <v>0.0386616125754874</v>
-      </c>
-      <c r="H9" s="5" t="n">
-        <v>0.0382965594583559</v>
-      </c>
-      <c r="I9" s="5" t="n">
-        <v>0.0369772943339069</v>
-      </c>
-      <c r="J9" s="5" t="n">
-        <v>0.396515596522007</v>
-      </c>
-      <c r="K9" s="5" t="n">
-        <v>0.408344051148392</v>
-      </c>
-      <c r="L9" s="5" t="n">
-        <v>0.369142787285043</v>
-      </c>
-      <c r="M9" s="5" t="n">
-        <v>0.502854257860951</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:M9">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M9"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>0.423538992639194</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>0.488311732314396</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>0.451994938393242</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>0.612125962396808</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>0.505562872328129</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>0.486014862353483</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <v>0.482174833113015</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>0.288064182715374</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <v>0.45236798978276</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>0.304945047879883</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>0.360645035553213</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>0.335097450693683</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>0.0440370781706982</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>0.368373889678204</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>0.458892991087051</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>0.450014318771457</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>0.588153206280568</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>0.362233947914272</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>0.378085637290039</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>0.337842755332675</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <v>0.503218447489921</v>
-      </c>
-      <c r="K3" s="5" t="n">
-        <v>0.285926631609546</v>
-      </c>
-      <c r="L3" s="5" t="n">
-        <v>0.287204723238003</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>0.41506363499817</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>0.0397413759440207</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0.0394474444902204</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>0.039533627805454</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>0.0395503876585529</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0.0384348754692067</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>0.0400103388324699</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>0.399512601407442</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>0.394140913435524</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>0.395436188276863</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>0.34506888821952</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <v>0.34397920405824</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>0.5188012073911</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>0.0404995712871189</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0.0395934873938042</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>0.0399953587906389</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>0.0392763255491709</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0.0385429535581762</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>0.0391830163553665</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>0.0394414601728049</v>
-      </c>
-      <c r="I5" s="5" t="n">
-        <v>0.254641566609901</v>
-      </c>
-      <c r="J5" s="5" t="n">
-        <v>0.409880561097697</v>
-      </c>
-      <c r="K5" s="5" t="n">
-        <v>0.563664357071781</v>
-      </c>
-      <c r="L5" s="5" t="n">
-        <v>0.351883699201556</v>
-      </c>
-      <c r="M5" s="5" t="n">
-        <v>0.290367979633172</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>0.0397341899111802</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>0.0385501199071268</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>0.0372924464949003</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>0.0387096017657734</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>0.0381549528984127</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>0.0397467655466825</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>0.296383672111385</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <v>0.339298925104208</v>
-      </c>
-      <c r="J6" s="5" t="n">
-        <v>0.405547605714917</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>0.378227920430886</v>
-      </c>
-      <c r="L6" s="5" t="n">
-        <v>0.392125001485235</v>
-      </c>
-      <c r="M6" s="5" t="n">
-        <v>0.484204735815363</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>0.0402380991078626</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>0.0381155752870734</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>0.0394025641194448</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>0.0391537118353301</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>0.0398509776802667</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <v>0.0395402119563223</v>
-      </c>
-      <c r="H7" s="5" t="n">
-        <v>0.0392302665825735</v>
-      </c>
-      <c r="I7" s="5" t="n">
-        <v>0.0413107763048406</v>
-      </c>
-      <c r="J7" s="5" t="n">
-        <v>0.381049249143666</v>
-      </c>
-      <c r="K7" s="5" t="n">
-        <v>0.601778101815888</v>
-      </c>
-      <c r="L7" s="5" t="n">
-        <v>0.464239253219776</v>
-      </c>
-      <c r="M7" s="5" t="n">
-        <v>0.348848327890818</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>0.0392745309525255</v>
-      </c>
-      <c r="C8" s="5" t="n">
-        <v>0.0394366727782432</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>0.039213519078473</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>0.0388488229424941</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>0.0392326591358807</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>0.0392428276344861</v>
-      </c>
-      <c r="H8" s="5" t="n">
-        <v>0.0396677247435611</v>
-      </c>
-      <c r="I8" s="5" t="n">
-        <v>0.0388769115942524</v>
-      </c>
-      <c r="J8" s="5" t="n">
-        <v>0.589102664878692</v>
-      </c>
-      <c r="K8" s="5" t="n">
-        <v>0.383648362595784</v>
-      </c>
-      <c r="L8" s="5" t="n">
-        <v>0.426899464737079</v>
-      </c>
-      <c r="M8" s="5" t="n">
-        <v>0.427136112806911</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>0.0377213993574357</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>0.0400229224669291</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>0.0405295666929271</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>0.0384856270232751</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>0.038568633522598</v>
-      </c>
-      <c r="G9" s="5" t="n">
-        <v>0.0387048224319293</v>
-      </c>
-      <c r="H9" s="5" t="n">
-        <v>0.0387257324058124</v>
-      </c>
-      <c r="I9" s="5" t="n">
-        <v>0.0390526563117933</v>
-      </c>
-      <c r="J9" s="5" t="n">
-        <v>0.446034185730248</v>
-      </c>
-      <c r="K9" s="5" t="n">
-        <v>0.432144613186851</v>
-      </c>
-      <c r="L9" s="5" t="n">
-        <v>0.471834721759773</v>
-      </c>
-      <c r="M9" s="5" t="n">
-        <v>0.746237781267078</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:M9">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M9"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="E1" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F1" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="G1" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="H1" s="0" t="n">
-        <v>7</v>
-      </c>
-      <c r="I1" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="J1" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="K1" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>11</v>
-      </c>
-      <c r="M1" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5" t="n">
-        <v>0.338153373460269</v>
-      </c>
-      <c r="C2" s="5" t="n">
-        <v>0.554603883751092</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>0.537996591121118</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>0.514096797160892</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>0.50217268346036</v>
-      </c>
-      <c r="G2" s="5" t="n">
-        <v>0.479205865183706</v>
-      </c>
-      <c r="H2" s="5" t="n">
-        <v>0.646437906025183</v>
-      </c>
-      <c r="I2" s="5" t="n">
-        <v>0.376440385611703</v>
-      </c>
-      <c r="J2" s="5" t="n">
-        <v>0.558790202009899</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>0.540711838342408</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>0.569482927239416</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>0.477927138475242</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="n">
-        <v>0.0408012989152388</v>
-      </c>
-      <c r="C3" s="5" t="n">
-        <v>0.0413836721194609</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>0.0423398763721745</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>0.181624646010517</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>0.377321287871159</v>
-      </c>
-      <c r="G3" s="5" t="n">
-        <v>0.52981533733745</v>
-      </c>
-      <c r="H3" s="5" t="n">
-        <v>0.526889734923352</v>
-      </c>
-      <c r="I3" s="5" t="n">
-        <v>0.5419849143909</v>
-      </c>
-      <c r="J3" s="5" t="n">
-        <v>0.507616012759637</v>
-      </c>
-      <c r="K3" s="5" t="n">
-        <v>0.3964904369002</v>
-      </c>
-      <c r="L3" s="5" t="n">
-        <v>0.415487840806478</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>0.540622137454392</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="n">
-        <v>0.0399677628324548</v>
-      </c>
-      <c r="C4" s="5" t="n">
-        <v>0.0402287493324903</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>0.0393782577331568</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>0.0391105651657672</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>0.0387264590222155</v>
-      </c>
-      <c r="G4" s="5" t="n">
-        <v>0.0377433976524823</v>
-      </c>
-      <c r="H4" s="5" t="n">
-        <v>0.0400213939049781</v>
-      </c>
-      <c r="I4" s="5" t="n">
-        <v>0.11748191877229</v>
-      </c>
-      <c r="J4" s="5" t="n">
-        <v>0.286412601090833</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>0.400712131636769</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <v>0.526715969805007</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>0.463132419395305</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>0.0399882503255867</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>0.0381218348861506</v>
-      </c>
-      <c r="D5" s="5" t="n">
-        <v>0.0413449841265705</v>
-      </c>
-      <c r="E5" s="5" t="n">
-        <v>0.0394570930591579</v>
-      </c>
-      <c r="F5" s="5" t="n">
-        <v>0.0411352826437749</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <v>0.0390630594571304</v>
-      </c>
-      <c r="H5" s="5" t="n">
-        <v>0.0384087312666514</v>
-      </c>
-      <c r="I5" s="5" t="n">
-        <v>0.0388803011367327</v>
-      </c>
-      <c r="J5" s="5" t="n">
-        <v>0.464744663217354</v>
-      </c>
-      <c r="K5" s="5" t="n">
-        <v>0.460906251430879</v>
-      </c>
-      <c r="L5" s="5" t="n">
-        <v>0.505162728791778</v>
-      </c>
-      <c r="M5" s="5" t="n">
-        <v>0.494961601003546</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>0.0435387074468432</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>0.0394276033611212</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>0.0374413643675347</v>
-      </c>
-      <c r="E6" s="5" t="n">
-        <v>0.0376450939239616</v>
-      </c>
-      <c r="F6" s="5" t="n">
-        <v>0.0369671646161863</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <v>0.0390257801350154</v>
-      </c>
-      <c r="H6" s="5" t="n">
-        <v>0.0378777021214141</v>
-      </c>
-      <c r="I6" s="5" t="n">
-        <v>0.0392982334516857</v>
-      </c>
-      <c r="J6" s="5" t="n">
-        <v>0.209296995440488</v>
-      </c>
-      <c r="K6" s="5" t="n">
-        <v>0.481047016824626</v>
-      </c>
-      <c r="L6" s="5" t="n">
-        <v>0.582657833930603</v>
-      </c>
-      <c r="M6" s="5" t="n">
-        <v>0.466313056903085</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="5" t="n">
-        <v>0.0409413837821215</v>
-      </c>
-      <c r="C7" s="5" t="n">
-        <v>0.0388905191445103</v>
-      </c>
-      <c r="D7" s="5" t="n">
-        <v>0.0396099901257659</v>
-      </c>
-      <c r="E7" s="5" t="n">
-        <v>0.0381410354203052</v>
-      </c>
-      <c r="F7" s="5" t="n">
-        <v>0.0379328749199118</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <v>0.0383631032693955</v>
-      </c>
-      <c r="H7" s="5" t="n">
-        <v>0.0394077440805766</v>
-      </c>
-      <c r="I7" s="5" t="n">
-        <v>0.040038870628971</v>
-      </c>
-      <c r="J7" s="5" t="n">
-        <v>0.039550991966244</v>
-      </c>
-      <c r="K7" s="5" t="n">
-        <v>0.505699467364757</v>
-      </c>
-      <c r="L7" s="5" t="n">
-        <v>0.508139856208004</v>
-      </c>
-      <c r="M7" s="5" t="n">
-        <v>0.476411775592257</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="n">
-        <v>0.041343775182324</v>
-      </c>
-      <c r="C8" s="5" t="n">
-        <v>0.0397009111447857</v>
-      </c>
-      <c r="D8" s="5" t="n">
-        <v>0.0400316387958135</v>
-      </c>
-      <c r="E8" s="5" t="n">
-        <v>0.0391213899782058</v>
-      </c>
-      <c r="F8" s="5" t="n">
-        <v>0.0383024734800633</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <v>0.0397816119664764</v>
-      </c>
-      <c r="H8" s="5" t="n">
-        <v>0.0390155589443817</v>
-      </c>
-      <c r="I8" s="5" t="n">
-        <v>0.0397328283338832</v>
-      </c>
-      <c r="J8" s="5" t="n">
-        <v>0.46651734864765</v>
-      </c>
-      <c r="K8" s="5" t="n">
-        <v>0.496083107326997</v>
-      </c>
-      <c r="L8" s="5" t="n">
-        <v>0.50731367468521</v>
-      </c>
-      <c r="M8" s="5" t="n">
-        <v>0.545987018735033</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="n">
-        <v>0.0386795960826078</v>
-      </c>
-      <c r="C9" s="5" t="n">
-        <v>0.0397707706856615</v>
-      </c>
-      <c r="D9" s="5" t="n">
-        <v>0.038533031837442</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>0.0387577037915165</v>
-      </c>
-      <c r="F9" s="5" t="n">
-        <v>0.038402126917703</v>
-      </c>
-      <c r="G9" s="5" t="n">
-        <v>0.0379256780704267</v>
-      </c>
-      <c r="H9" s="5" t="n">
-        <v>0.0394992246731085</v>
-      </c>
-      <c r="I9" s="5" t="n">
-        <v>0.0387240556715275</v>
-      </c>
-      <c r="J9" s="5" t="n">
-        <v>0.0386795960826078</v>
-      </c>
-      <c r="K9" s="5" t="n">
-        <v>0.579645234104184</v>
-      </c>
-      <c r="L9" s="5" t="n">
-        <v>0.555661502821253</v>
-      </c>
-      <c r="M9" s="5" t="n">
-        <v>0.682762942722486</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B2:M9">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFFEF9C"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>